<commit_message>
Deleted unused files. Uploaded new data file
</commit_message>
<xml_diff>
--- a/formulation/data/FDA_APPROVED.xlsx
+++ b/formulation/data/FDA_APPROVED.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawei\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawei\Desktop\project\formulation\formulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911F8A60-63FA-4757-82FF-07062D08834E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337F06A8-BA6B-4CF7-ABD5-35DF3B86DAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,17 @@
     <sheet name="BDDCSTable" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BDDCSTable!$E$1:$E$928</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3187,10 +3192,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>39 (60000)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Pyrantel Pamoate</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3358,6 +3359,9 @@
   </si>
   <si>
     <t>Dantrolene</t>
+  </si>
+  <si>
+    <t>39 (60000)</t>
   </si>
 </sst>
 </file>
@@ -3869,10 +3873,10 @@
   <sheetPr published="0"/>
   <dimension ref="A1:Y928"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1380" activePane="bottomLeft"/>
-      <selection activeCell="G841" sqref="G841"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1380" topLeftCell="A791" activePane="bottomLeft"/>
+      <selection activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="C797" sqref="C797"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5200,7 +5204,7 @@
     </row>
     <row r="19" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B19" s="13">
         <v>1</v>
@@ -5274,7 +5278,7 @@
     </row>
     <row r="20" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B20" s="13">
         <v>1</v>
@@ -5352,7 +5356,7 @@
     </row>
     <row r="21" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B21" s="13">
         <v>1</v>
@@ -5424,7 +5428,7 @@
     </row>
     <row r="22" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B22" s="13">
         <v>1</v>
@@ -5490,7 +5494,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B23" s="13">
         <v>1</v>
@@ -5502,7 +5506,7 @@
         <v>992</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>994</v>
@@ -5552,7 +5556,7 @@
     </row>
     <row r="24" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B24" s="13">
         <v>1</v>
@@ -7454,7 +7458,7 @@
     </row>
     <row r="50" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B50" s="13">
         <v>1</v>
@@ -7524,7 +7528,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B51" s="13">
         <v>1</v>
@@ -7539,7 +7543,7 @@
         <v>993</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G51" s="16">
         <v>0.16999999999999998</v>
@@ -7592,7 +7596,7 @@
     </row>
     <row r="52" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B52" s="13">
         <v>1</v>
@@ -7668,7 +7672,7 @@
     </row>
     <row r="53" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B53" s="13">
         <v>1</v>
@@ -7744,7 +7748,7 @@
     </row>
     <row r="54" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B54" s="13">
         <v>1</v>
@@ -7822,7 +7826,7 @@
     </row>
     <row r="55" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B55" s="13">
         <v>1</v>
@@ -7894,7 +7898,7 @@
     </row>
     <row r="56" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B56" s="13">
         <v>1</v>
@@ -7962,7 +7966,7 @@
     </row>
     <row r="57" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B57" s="13">
         <v>1</v>
@@ -8038,7 +8042,7 @@
     </row>
     <row r="58" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B58" s="13">
         <v>1</v>
@@ -8050,7 +8054,7 @@
         <v>982</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F58" s="15" t="s">
         <v>984</v>
@@ -8116,7 +8120,7 @@
     </row>
     <row r="59" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B59" s="13">
         <v>1</v>
@@ -8190,7 +8194,7 @@
     </row>
     <row r="60" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B60" s="13">
         <v>1</v>
@@ -8258,7 +8262,7 @@
     </row>
     <row r="61" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B61" s="13">
         <v>1</v>
@@ -8674,7 +8678,7 @@
     </row>
     <row r="67" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B67" s="13">
         <v>1</v>
@@ -8742,7 +8746,7 @@
     </row>
     <row r="68" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B68" s="13">
         <v>1</v>
@@ -8818,7 +8822,7 @@
     </row>
     <row r="69" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="13" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B69" s="13">
         <v>1</v>
@@ -8896,7 +8900,7 @@
     </row>
     <row r="70" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="13" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B70" s="13">
         <v>1</v>
@@ -8974,7 +8978,7 @@
     </row>
     <row r="71" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A71" s="13" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B71" s="13">
         <v>1</v>
@@ -9052,7 +9056,7 @@
     </row>
     <row r="72" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="13" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B72" s="13">
         <v>1</v>
@@ -9130,7 +9134,7 @@
     </row>
     <row r="73" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A73" s="13" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B73" s="13">
         <v>1</v>
@@ -9202,7 +9206,7 @@
     </row>
     <row r="74" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B74" s="13">
         <v>1</v>
@@ -9280,7 +9284,7 @@
     </row>
     <row r="75" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A75" s="13" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B75" s="13">
         <v>1</v>
@@ -9356,7 +9360,7 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B76" s="13">
         <v>1</v>
@@ -9420,7 +9424,7 @@
     </row>
     <row r="77" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B77" s="13">
         <v>1</v>
@@ -9498,7 +9502,7 @@
     </row>
     <row r="78" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B78" s="13">
         <v>1</v>
@@ -9574,7 +9578,7 @@
     </row>
     <row r="79" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B79" s="13">
         <v>1</v>
@@ -9650,14 +9654,14 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B80" s="13">
         <v>1</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E80" s="15"/>
       <c r="F80" s="15"/>
@@ -9714,7 +9718,7 @@
     </row>
     <row r="81" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A81" s="13" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B81" s="13">
         <v>1</v>
@@ -9790,7 +9794,7 @@
     </row>
     <row r="82" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="13" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B82" s="13">
         <v>1</v>
@@ -9860,7 +9864,7 @@
     </row>
     <row r="83" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="13" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B83" s="13">
         <v>1</v>
@@ -9938,7 +9942,7 @@
     </row>
     <row r="84" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" s="13" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B84" s="13">
         <v>1</v>
@@ -10008,7 +10012,7 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B85" s="13">
         <v>1</v>
@@ -10023,7 +10027,7 @@
         <v>993</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G85" s="16">
         <v>1.6</v>
@@ -10078,7 +10082,7 @@
     </row>
     <row r="86" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A86" s="13" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B86" s="13">
         <v>1</v>
@@ -10156,7 +10160,7 @@
     </row>
     <row r="87" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A87" s="13" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B87" s="13">
         <v>1</v>
@@ -10232,7 +10236,7 @@
     </row>
     <row r="88" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="13" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B88" s="13">
         <v>1</v>
@@ -10308,7 +10312,7 @@
     </row>
     <row r="89" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A89" s="13" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B89" s="13">
         <v>1</v>
@@ -10382,7 +10386,7 @@
     </row>
     <row r="90" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A90" s="13" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B90" s="13">
         <v>1</v>
@@ -10456,7 +10460,7 @@
     </row>
     <row r="91" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A91" s="13" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B91" s="13">
         <v>1</v>
@@ -10530,7 +10534,7 @@
     </row>
     <row r="92" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A92" s="13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B92" s="13">
         <v>1</v>
@@ -10608,7 +10612,7 @@
     </row>
     <row r="93" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B93" s="13">
         <v>1</v>
@@ -10684,7 +10688,7 @@
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B94" s="13">
         <v>1</v>
@@ -10750,7 +10754,7 @@
     </row>
     <row r="95" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A95" s="13" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B95" s="13">
         <v>1</v>
@@ -10826,7 +10830,7 @@
     </row>
     <row r="96" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A96" s="13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B96" s="13">
         <v>1</v>
@@ -11057,7 +11061,7 @@
       </c>
       <c r="C99" s="15"/>
       <c r="D99" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E99" s="15"/>
       <c r="F99" s="15"/>
@@ -14075,7 +14079,7 @@
       </c>
       <c r="C141" s="15"/>
       <c r="D141" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E141" s="15"/>
       <c r="F141" s="15"/>
@@ -16260,7 +16264,7 @@
         <v>996</v>
       </c>
       <c r="E171" s="13" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F171" s="15" t="s">
         <v>967</v>
@@ -17559,7 +17563,7 @@
         <v>993</v>
       </c>
       <c r="F189" s="15" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G189" s="16">
         <v>0.16999999999999998</v>
@@ -18439,7 +18443,7 @@
         <v>993</v>
       </c>
       <c r="F201" s="15" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G201" s="16">
         <v>2.4</v>
@@ -19890,10 +19894,10 @@
         <v>997</v>
       </c>
       <c r="E221" s="13" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F221" s="15" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G221" s="16">
         <v>1</v>
@@ -20995,7 +20999,7 @@
       </c>
       <c r="C236" s="15"/>
       <c r="D236" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E236" s="15"/>
       <c r="F236" s="15"/>
@@ -25037,7 +25041,7 @@
         <v>993</v>
       </c>
       <c r="F291" s="15" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G291" s="16">
         <v>53.8</v>
@@ -28284,7 +28288,7 @@
         <v>982</v>
       </c>
       <c r="E335" s="15" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F335" s="15" t="s">
         <v>984</v>
@@ -29591,7 +29595,7 @@
       </c>
       <c r="C353" s="13"/>
       <c r="D353" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E353" s="15"/>
       <c r="F353" s="15"/>
@@ -29653,7 +29657,7 @@
       </c>
       <c r="C354" s="15"/>
       <c r="D354" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E354" s="15"/>
       <c r="F354" s="15"/>
@@ -29915,7 +29919,7 @@
       </c>
       <c r="C358" s="15"/>
       <c r="D358" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E358" s="15"/>
       <c r="F358" s="15"/>
@@ -31875,7 +31879,7 @@
       </c>
       <c r="C386" s="15"/>
       <c r="D386" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E386" s="15"/>
       <c r="F386" s="15"/>
@@ -33704,7 +33708,7 @@
         <v>982</v>
       </c>
       <c r="E411" s="15" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F411" s="15" t="s">
         <v>984</v>
@@ -40235,7 +40239,7 @@
       </c>
       <c r="C500" s="15"/>
       <c r="D500" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E500" s="15"/>
       <c r="F500" s="15"/>
@@ -43794,7 +43798,7 @@
     </row>
     <row r="549" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A549" s="13" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B549" s="13">
         <v>2</v>
@@ -45009,7 +45013,7 @@
       </c>
       <c r="C566" s="15"/>
       <c r="D566" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E566" s="15"/>
       <c r="F566" s="15"/>
@@ -45519,7 +45523,7 @@
       </c>
       <c r="C573" s="15"/>
       <c r="D573" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E573" s="15"/>
       <c r="F573" s="15"/>
@@ -48812,7 +48816,7 @@
       </c>
       <c r="C619" s="15"/>
       <c r="D619" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E619" s="15"/>
       <c r="F619" s="15"/>
@@ -50266,7 +50270,7 @@
       </c>
       <c r="C639" s="15"/>
       <c r="D639" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E639" s="15"/>
       <c r="F639" s="15"/>
@@ -53784,7 +53788,7 @@
       </c>
       <c r="C689" s="15"/>
       <c r="D689" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E689" s="15"/>
       <c r="F689" s="15"/>
@@ -55830,7 +55834,7 @@
       </c>
       <c r="C718" s="15"/>
       <c r="D718" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E718" s="15"/>
       <c r="F718" s="15"/>
@@ -56968,7 +56972,7 @@
       </c>
       <c r="C734" s="15"/>
       <c r="D734" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E734" s="15"/>
       <c r="F734" s="15"/>
@@ -57324,7 +57328,7 @@
       </c>
       <c r="C739" s="15"/>
       <c r="D739" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E739" s="15"/>
       <c r="F739" s="15"/>
@@ -57641,7 +57645,7 @@
         <v>941</v>
       </c>
       <c r="E744" s="13" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F744" s="15" t="s">
         <v>967</v>
@@ -58141,7 +58145,7 @@
         <v>1012</v>
       </c>
       <c r="E751" s="13" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F751" s="15" t="s">
         <v>967</v>
@@ -59950,7 +59954,7 @@
       </c>
       <c r="C776" s="15"/>
       <c r="D776" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E776" s="15"/>
       <c r="F776" s="15"/>
@@ -60738,7 +60742,7 @@
       </c>
       <c r="C787" s="15"/>
       <c r="D787" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E787" s="15"/>
       <c r="F787" s="15"/>
@@ -60864,7 +60868,7 @@
       </c>
       <c r="C789" s="15"/>
       <c r="D789" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E789" s="15"/>
       <c r="F789" s="15"/>
@@ -61379,7 +61383,7 @@
         <v>3</v>
       </c>
       <c r="C797" s="13" t="s">
-        <v>1017</v>
+        <v>1072</v>
       </c>
       <c r="D797" s="13" t="s">
         <v>1014</v>
@@ -62756,7 +62760,7 @@
       </c>
       <c r="C816" s="15"/>
       <c r="D816" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E816" s="15"/>
       <c r="F816" s="15"/>
@@ -62874,7 +62878,7 @@
       </c>
       <c r="C818" s="15"/>
       <c r="D818" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E818" s="15"/>
       <c r="F818" s="15"/>
@@ -63418,7 +63422,7 @@
       </c>
       <c r="C826" s="15"/>
       <c r="D826" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E826" s="15"/>
       <c r="F826" s="15"/>
@@ -64192,7 +64196,7 @@
       </c>
       <c r="C837" s="15"/>
       <c r="D837" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E837" s="15"/>
       <c r="F837" s="15"/>
@@ -64468,7 +64472,7 @@
         <v>240</v>
       </c>
       <c r="F841" s="15" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="G841" s="16">
         <v>1.7</v>
@@ -66586,7 +66590,7 @@
       </c>
       <c r="C871" s="15"/>
       <c r="D871" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E871" s="15"/>
       <c r="F871" s="15"/>
@@ -66784,7 +66788,7 @@
       </c>
       <c r="C874" s="13"/>
       <c r="D874" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E874" s="15"/>
       <c r="F874" s="15"/>
@@ -67648,7 +67652,7 @@
       </c>
       <c r="C886" s="15"/>
       <c r="D886" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E886" s="15"/>
       <c r="F886" s="15"/>
@@ -68082,7 +68086,7 @@
       </c>
       <c r="C892" s="15"/>
       <c r="D892" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E892" s="15"/>
       <c r="F892" s="15"/>
@@ -69674,7 +69678,7 @@
       </c>
       <c r="C914" s="15"/>
       <c r="D914" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E914" s="15"/>
       <c r="F914" s="15"/>
@@ -69728,7 +69732,7 @@
       </c>
       <c r="C915" s="15"/>
       <c r="D915" s="15" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E915" s="15"/>
       <c r="F915" s="15"/>
@@ -70719,6 +70723,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E928" xr:uid="{0E26623D-527A-4B55-944B-59514BD3DBC3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y928">
     <sortCondition ref="H3:H928"/>
     <sortCondition ref="F3:F928"/>

</xml_diff>

<commit_message>
Predict on missing value using RandomForestRegressor.
</commit_message>
<xml_diff>
--- a/formulation/data/FDA_APPROVED.xlsx
+++ b/formulation/data/FDA_APPROVED.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawei\Desktop\project\formulation\formulation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawei\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337F06A8-BA6B-4CF7-ABD5-35DF3B86DAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911F8A60-63FA-4757-82FF-07062D08834E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,12 @@
     <sheet name="BDDCSTable" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BDDCSTable!$E$1:$E$928</definedName>
-  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3192,6 +3187,10 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>39 (60000)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Pyrantel Pamoate</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -3359,9 +3358,6 @@
   </si>
   <si>
     <t>Dantrolene</t>
-  </si>
-  <si>
-    <t>39 (60000)</t>
   </si>
 </sst>
 </file>
@@ -3873,10 +3869,10 @@
   <sheetPr published="0"/>
   <dimension ref="A1:Y928"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1380" topLeftCell="A791" activePane="bottomLeft"/>
-      <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="C797" sqref="C797"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1380" activePane="bottomLeft"/>
+      <selection activeCell="G841" sqref="G841"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5204,7 +5200,7 @@
     </row>
     <row r="19" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B19" s="13">
         <v>1</v>
@@ -5278,7 +5274,7 @@
     </row>
     <row r="20" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B20" s="13">
         <v>1</v>
@@ -5356,7 +5352,7 @@
     </row>
     <row r="21" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B21" s="13">
         <v>1</v>
@@ -5428,7 +5424,7 @@
     </row>
     <row r="22" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B22" s="13">
         <v>1</v>
@@ -5494,7 +5490,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B23" s="13">
         <v>1</v>
@@ -5506,7 +5502,7 @@
         <v>992</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>994</v>
@@ -5556,7 +5552,7 @@
     </row>
     <row r="24" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B24" s="13">
         <v>1</v>
@@ -7458,7 +7454,7 @@
     </row>
     <row r="50" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B50" s="13">
         <v>1</v>
@@ -7528,7 +7524,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B51" s="13">
         <v>1</v>
@@ -7543,7 +7539,7 @@
         <v>993</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="G51" s="16">
         <v>0.16999999999999998</v>
@@ -7596,7 +7592,7 @@
     </row>
     <row r="52" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B52" s="13">
         <v>1</v>
@@ -7672,7 +7668,7 @@
     </row>
     <row r="53" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B53" s="13">
         <v>1</v>
@@ -7748,7 +7744,7 @@
     </row>
     <row r="54" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B54" s="13">
         <v>1</v>
@@ -7826,7 +7822,7 @@
     </row>
     <row r="55" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B55" s="13">
         <v>1</v>
@@ -7898,7 +7894,7 @@
     </row>
     <row r="56" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B56" s="13">
         <v>1</v>
@@ -7966,7 +7962,7 @@
     </row>
     <row r="57" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B57" s="13">
         <v>1</v>
@@ -8042,7 +8038,7 @@
     </row>
     <row r="58" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B58" s="13">
         <v>1</v>
@@ -8054,7 +8050,7 @@
         <v>982</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F58" s="15" t="s">
         <v>984</v>
@@ -8120,7 +8116,7 @@
     </row>
     <row r="59" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B59" s="13">
         <v>1</v>
@@ -8194,7 +8190,7 @@
     </row>
     <row r="60" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B60" s="13">
         <v>1</v>
@@ -8262,7 +8258,7 @@
     </row>
     <row r="61" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B61" s="13">
         <v>1</v>
@@ -8678,7 +8674,7 @@
     </row>
     <row r="67" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B67" s="13">
         <v>1</v>
@@ -8746,7 +8742,7 @@
     </row>
     <row r="68" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B68" s="13">
         <v>1</v>
@@ -8822,7 +8818,7 @@
     </row>
     <row r="69" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="13" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B69" s="13">
         <v>1</v>
@@ -8900,7 +8896,7 @@
     </row>
     <row r="70" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="13" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B70" s="13">
         <v>1</v>
@@ -8978,7 +8974,7 @@
     </row>
     <row r="71" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A71" s="13" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B71" s="13">
         <v>1</v>
@@ -9056,7 +9052,7 @@
     </row>
     <row r="72" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="13" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B72" s="13">
         <v>1</v>
@@ -9134,7 +9130,7 @@
     </row>
     <row r="73" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A73" s="13" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B73" s="13">
         <v>1</v>
@@ -9206,7 +9202,7 @@
     </row>
     <row r="74" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B74" s="13">
         <v>1</v>
@@ -9284,7 +9280,7 @@
     </row>
     <row r="75" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A75" s="13" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B75" s="13">
         <v>1</v>
@@ -9360,7 +9356,7 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B76" s="13">
         <v>1</v>
@@ -9424,7 +9420,7 @@
     </row>
     <row r="77" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B77" s="13">
         <v>1</v>
@@ -9502,7 +9498,7 @@
     </row>
     <row r="78" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B78" s="13">
         <v>1</v>
@@ -9578,7 +9574,7 @@
     </row>
     <row r="79" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B79" s="13">
         <v>1</v>
@@ -9654,14 +9650,14 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B80" s="13">
         <v>1</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E80" s="15"/>
       <c r="F80" s="15"/>
@@ -9718,7 +9714,7 @@
     </row>
     <row r="81" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A81" s="13" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B81" s="13">
         <v>1</v>
@@ -9794,7 +9790,7 @@
     </row>
     <row r="82" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="13" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="B82" s="13">
         <v>1</v>
@@ -9864,7 +9860,7 @@
     </row>
     <row r="83" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="13" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B83" s="13">
         <v>1</v>
@@ -9942,7 +9938,7 @@
     </row>
     <row r="84" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" s="13" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B84" s="13">
         <v>1</v>
@@ -10012,7 +10008,7 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B85" s="13">
         <v>1</v>
@@ -10027,7 +10023,7 @@
         <v>993</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="G85" s="16">
         <v>1.6</v>
@@ -10082,7 +10078,7 @@
     </row>
     <row r="86" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A86" s="13" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B86" s="13">
         <v>1</v>
@@ -10160,7 +10156,7 @@
     </row>
     <row r="87" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A87" s="13" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B87" s="13">
         <v>1</v>
@@ -10236,7 +10232,7 @@
     </row>
     <row r="88" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="13" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B88" s="13">
         <v>1</v>
@@ -10312,7 +10308,7 @@
     </row>
     <row r="89" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A89" s="13" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B89" s="13">
         <v>1</v>
@@ -10386,7 +10382,7 @@
     </row>
     <row r="90" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A90" s="13" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="B90" s="13">
         <v>1</v>
@@ -10460,7 +10456,7 @@
     </row>
     <row r="91" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A91" s="13" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B91" s="13">
         <v>1</v>
@@ -10534,7 +10530,7 @@
     </row>
     <row r="92" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A92" s="13" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B92" s="13">
         <v>1</v>
@@ -10612,7 +10608,7 @@
     </row>
     <row r="93" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B93" s="13">
         <v>1</v>
@@ -10688,7 +10684,7 @@
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="B94" s="13">
         <v>1</v>
@@ -10754,7 +10750,7 @@
     </row>
     <row r="95" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A95" s="13" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B95" s="13">
         <v>1</v>
@@ -10830,7 +10826,7 @@
     </row>
     <row r="96" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A96" s="13" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B96" s="13">
         <v>1</v>
@@ -11061,7 +11057,7 @@
       </c>
       <c r="C99" s="15"/>
       <c r="D99" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E99" s="15"/>
       <c r="F99" s="15"/>
@@ -14079,7 +14075,7 @@
       </c>
       <c r="C141" s="15"/>
       <c r="D141" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E141" s="15"/>
       <c r="F141" s="15"/>
@@ -16264,7 +16260,7 @@
         <v>996</v>
       </c>
       <c r="E171" s="13" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F171" s="15" t="s">
         <v>967</v>
@@ -17563,7 +17559,7 @@
         <v>993</v>
       </c>
       <c r="F189" s="15" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="G189" s="16">
         <v>0.16999999999999998</v>
@@ -18443,7 +18439,7 @@
         <v>993</v>
       </c>
       <c r="F201" s="15" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="G201" s="16">
         <v>2.4</v>
@@ -19894,10 +19890,10 @@
         <v>997</v>
       </c>
       <c r="E221" s="13" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F221" s="15" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="G221" s="16">
         <v>1</v>
@@ -20999,7 +20995,7 @@
       </c>
       <c r="C236" s="15"/>
       <c r="D236" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E236" s="15"/>
       <c r="F236" s="15"/>
@@ -25041,7 +25037,7 @@
         <v>993</v>
       </c>
       <c r="F291" s="15" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="G291" s="16">
         <v>53.8</v>
@@ -28288,7 +28284,7 @@
         <v>982</v>
       </c>
       <c r="E335" s="15" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F335" s="15" t="s">
         <v>984</v>
@@ -29595,7 +29591,7 @@
       </c>
       <c r="C353" s="13"/>
       <c r="D353" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E353" s="15"/>
       <c r="F353" s="15"/>
@@ -29657,7 +29653,7 @@
       </c>
       <c r="C354" s="15"/>
       <c r="D354" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E354" s="15"/>
       <c r="F354" s="15"/>
@@ -29919,7 +29915,7 @@
       </c>
       <c r="C358" s="15"/>
       <c r="D358" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E358" s="15"/>
       <c r="F358" s="15"/>
@@ -31879,7 +31875,7 @@
       </c>
       <c r="C386" s="15"/>
       <c r="D386" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E386" s="15"/>
       <c r="F386" s="15"/>
@@ -33708,7 +33704,7 @@
         <v>982</v>
       </c>
       <c r="E411" s="15" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F411" s="15" t="s">
         <v>984</v>
@@ -40239,7 +40235,7 @@
       </c>
       <c r="C500" s="15"/>
       <c r="D500" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E500" s="15"/>
       <c r="F500" s="15"/>
@@ -43798,7 +43794,7 @@
     </row>
     <row r="549" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A549" s="13" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B549" s="13">
         <v>2</v>
@@ -45013,7 +45009,7 @@
       </c>
       <c r="C566" s="15"/>
       <c r="D566" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E566" s="15"/>
       <c r="F566" s="15"/>
@@ -45523,7 +45519,7 @@
       </c>
       <c r="C573" s="15"/>
       <c r="D573" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E573" s="15"/>
       <c r="F573" s="15"/>
@@ -48816,7 +48812,7 @@
       </c>
       <c r="C619" s="15"/>
       <c r="D619" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E619" s="15"/>
       <c r="F619" s="15"/>
@@ -50270,7 +50266,7 @@
       </c>
       <c r="C639" s="15"/>
       <c r="D639" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E639" s="15"/>
       <c r="F639" s="15"/>
@@ -53788,7 +53784,7 @@
       </c>
       <c r="C689" s="15"/>
       <c r="D689" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E689" s="15"/>
       <c r="F689" s="15"/>
@@ -55834,7 +55830,7 @@
       </c>
       <c r="C718" s="15"/>
       <c r="D718" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E718" s="15"/>
       <c r="F718" s="15"/>
@@ -56972,7 +56968,7 @@
       </c>
       <c r="C734" s="15"/>
       <c r="D734" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E734" s="15"/>
       <c r="F734" s="15"/>
@@ -57328,7 +57324,7 @@
       </c>
       <c r="C739" s="15"/>
       <c r="D739" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E739" s="15"/>
       <c r="F739" s="15"/>
@@ -57645,7 +57641,7 @@
         <v>941</v>
       </c>
       <c r="E744" s="13" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F744" s="15" t="s">
         <v>967</v>
@@ -58145,7 +58141,7 @@
         <v>1012</v>
       </c>
       <c r="E751" s="13" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F751" s="15" t="s">
         <v>967</v>
@@ -59954,7 +59950,7 @@
       </c>
       <c r="C776" s="15"/>
       <c r="D776" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E776" s="15"/>
       <c r="F776" s="15"/>
@@ -60742,7 +60738,7 @@
       </c>
       <c r="C787" s="15"/>
       <c r="D787" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E787" s="15"/>
       <c r="F787" s="15"/>
@@ -60868,7 +60864,7 @@
       </c>
       <c r="C789" s="15"/>
       <c r="D789" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E789" s="15"/>
       <c r="F789" s="15"/>
@@ -61383,7 +61379,7 @@
         <v>3</v>
       </c>
       <c r="C797" s="13" t="s">
-        <v>1072</v>
+        <v>1017</v>
       </c>
       <c r="D797" s="13" t="s">
         <v>1014</v>
@@ -62760,7 +62756,7 @@
       </c>
       <c r="C816" s="15"/>
       <c r="D816" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E816" s="15"/>
       <c r="F816" s="15"/>
@@ -62878,7 +62874,7 @@
       </c>
       <c r="C818" s="15"/>
       <c r="D818" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E818" s="15"/>
       <c r="F818" s="15"/>
@@ -63422,7 +63418,7 @@
       </c>
       <c r="C826" s="15"/>
       <c r="D826" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E826" s="15"/>
       <c r="F826" s="15"/>
@@ -64196,7 +64192,7 @@
       </c>
       <c r="C837" s="15"/>
       <c r="D837" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E837" s="15"/>
       <c r="F837" s="15"/>
@@ -64472,7 +64468,7 @@
         <v>240</v>
       </c>
       <c r="F841" s="15" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="G841" s="16">
         <v>1.7</v>
@@ -66590,7 +66586,7 @@
       </c>
       <c r="C871" s="15"/>
       <c r="D871" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E871" s="15"/>
       <c r="F871" s="15"/>
@@ -66788,7 +66784,7 @@
       </c>
       <c r="C874" s="13"/>
       <c r="D874" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E874" s="15"/>
       <c r="F874" s="15"/>
@@ -67652,7 +67648,7 @@
       </c>
       <c r="C886" s="15"/>
       <c r="D886" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E886" s="15"/>
       <c r="F886" s="15"/>
@@ -68086,7 +68082,7 @@
       </c>
       <c r="C892" s="15"/>
       <c r="D892" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E892" s="15"/>
       <c r="F892" s="15"/>
@@ -69678,7 +69674,7 @@
       </c>
       <c r="C914" s="15"/>
       <c r="D914" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E914" s="15"/>
       <c r="F914" s="15"/>
@@ -69732,7 +69728,7 @@
       </c>
       <c r="C915" s="15"/>
       <c r="D915" s="15" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E915" s="15"/>
       <c r="F915" s="15"/>
@@ -70723,7 +70719,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E928" xr:uid="{0E26623D-527A-4B55-944B-59514BD3DBC3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y928">
     <sortCondition ref="H3:H928"/>
     <sortCondition ref="F3:F928"/>

</xml_diff>